<commit_message>
First Lecture Link Working
</commit_message>
<xml_diff>
--- a/My_Folder/sampleTT.xlsx
+++ b/My_Folder/sampleTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Desktop\SDP_Works\Time_Table_Linker_Project\My_Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26621C29-7DE7-42AA-A427-670586D9A190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278B8870-B78B-4BA0-A851-5D9B0ECCA248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
   <si>
     <t>Monday</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Saturday</t>
   </si>
   <si>
-    <t>https://meet.google.com/new</t>
-  </si>
-  <si>
     <t>Links Table</t>
   </si>
   <si>
@@ -60,77 +57,130 @@
     <t>DDB</t>
   </si>
   <si>
+    <t>DDB DCAN Tut</t>
+  </si>
+  <si>
+    <t>RSP OOP Lab</t>
+  </si>
+  <si>
+    <t>SSK OOP TUT</t>
+  </si>
+  <si>
+    <t>SVP CAOS TUT</t>
+  </si>
+  <si>
+    <t>DS TUT</t>
+  </si>
+  <si>
+    <t>VDP DCAN LAB</t>
+  </si>
+  <si>
+    <t>AAB DS LAB</t>
+  </si>
+  <si>
+    <t>CAOS LAB</t>
+  </si>
+  <si>
+    <t>EDAI LAB</t>
+  </si>
+  <si>
+    <t>SDP LAB</t>
+  </si>
+  <si>
+    <t>9:00 : 10:00</t>
+  </si>
+  <si>
+    <t>10:00 : 11:00</t>
+  </si>
+  <si>
+    <t>11:00 : 12:00</t>
+  </si>
+  <si>
+    <t>12:00 : 13:00</t>
+  </si>
+  <si>
+    <t>13:00 : 14:00</t>
+  </si>
+  <si>
+    <t>14:00 : 15:00</t>
+  </si>
+  <si>
+    <t>15:00 : 16:00</t>
+  </si>
+  <si>
+    <t>16:00 : 17:00</t>
+  </si>
+  <si>
+    <t>17:00 : 18:00</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>https://meet.google.com/qnx-rvwj-sgx?pli=1&amp;authuser=1</t>
+  </si>
+  <si>
+    <t>https://meet.google.com/hwq-mqef-ewm?pli=1&amp;authuser=1</t>
+  </si>
+  <si>
     <t>AAB DS</t>
   </si>
   <si>
-    <t>DDB DCAN Tut</t>
-  </si>
-  <si>
-    <t>RSP OOP Lab</t>
-  </si>
-  <si>
-    <t>SSK OOP TUT</t>
-  </si>
-  <si>
-    <t>SVP CAOS TUT</t>
-  </si>
-  <si>
-    <t>DS TUT</t>
-  </si>
-  <si>
-    <t>VDP DCAN LAB</t>
-  </si>
-  <si>
-    <t>AAB DS LAB</t>
-  </si>
-  <si>
-    <t>CAOS LAB</t>
-  </si>
-  <si>
-    <t>EDAI LAB</t>
-  </si>
-  <si>
-    <t>SDP LAB</t>
-  </si>
-  <si>
-    <t>9:00 : 10:00</t>
-  </si>
-  <si>
-    <t>10:00 : 11:00</t>
-  </si>
-  <si>
-    <t>11:00 : 12:00</t>
-  </si>
-  <si>
-    <t>12:00 : 13:00</t>
-  </si>
-  <si>
-    <t>13:00 : 14:00</t>
-  </si>
-  <si>
-    <t>14:00 : 15:00</t>
-  </si>
-  <si>
-    <t>15:00 : 16:00</t>
-  </si>
-  <si>
-    <t>16:00 : 17:00</t>
-  </si>
-  <si>
-    <t>17:00 : 18:00</t>
-  </si>
-  <si>
-    <t>Time</t>
+    <t>https://meet.google.com/ozp-cjab-vwg?pli=1&amp;authuser=1</t>
+  </si>
+  <si>
+    <t>https://meet.google.com/tmc-imzs-rag?pli=1&amp;authuser=1</t>
+  </si>
+  <si>
+    <t>https://meet.google.com/zry-qpco-gbr?pli=1&amp;authuser=1</t>
+  </si>
+  <si>
+    <t>https://meet.google.com/ycb-jmtr-nve?pli=1&amp;authuser=1</t>
+  </si>
+  <si>
+    <t>https://meet.google.com/ufn-uuaf-drt?pli=1&amp;authuser=1</t>
+  </si>
+  <si>
+    <t>https://meet.google.com/ykr-oigv-rwd?pli=1&amp;authuser=1</t>
+  </si>
+  <si>
+    <t>https://meet.google.com/dfm-cbgj-pzs?pli=1&amp;authuser=1</t>
+  </si>
+  <si>
+    <t>https://meet.google.com/gfj-wxiq-uiz?pli=1&amp;authuser=1</t>
+  </si>
+  <si>
+    <t>https://timetablesysem2.netlify.app/#?pli=1&amp;authuser=1</t>
+  </si>
+  <si>
+    <t>DDB DCAN TUT</t>
+  </si>
+  <si>
+    <t>https://meet.google.com/new2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -168,18 +218,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -460,15 +513,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
@@ -478,34 +531,34 @@
   <sheetData>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -513,21 +566,21 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -537,21 +590,21 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -561,21 +614,21 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -586,14 +639,14 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -606,24 +659,24 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -632,17 +685,17 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -650,127 +703,131 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B13:C13"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C27" r:id="rId1" xr:uid="{401B2C1E-30EC-4089-B4BC-8B1D0882BA85}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Trying for friday lec 1 and empty string
</commit_message>
<xml_diff>
--- a/My_Folder/sampleTT.xlsx
+++ b/My_Folder/sampleTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Desktop\SDP_Works\Time_Table_Linker_Project\My_Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278B8870-B78B-4BA0-A851-5D9B0ECCA248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE57A39A-59E0-4481-89B8-9DA114E89673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
   <si>
     <t>Monday</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>https://meet.google.com/new2</t>
+  </si>
+  <si>
+    <t>XAB</t>
   </si>
 </sst>
 </file>
@@ -194,7 +197,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -217,19 +220,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -511,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A5:J27"/>
+  <dimension ref="A5:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -657,7 +672,9 @@
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
@@ -702,10 +719,10 @@
       <c r="J11" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
@@ -815,8 +832,16 @@
       <c r="B27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
After Ui First Commit
</commit_message>
<xml_diff>
--- a/My_Folder/sampleTT.xlsx
+++ b/My_Folder/sampleTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Desktop\SDP_Works\Time_Table_Linker_Project\My_Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE57A39A-59E0-4481-89B8-9DA114E89673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0F5E90-EBB6-4697-9EF4-59FDF502DC60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
   <si>
     <t>Monday</t>
   </si>
@@ -529,7 +529,7 @@
   <dimension ref="A5:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -672,9 +672,7 @@
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>